<commit_message>
updating UCLA VAT analyses
</commit_message>
<xml_diff>
--- a/UCLA_VAT/UCLA_VAT.xlsx
+++ b/UCLA_VAT/UCLA_VAT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10514"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twwebb/Documents/python/GPT3_analogies_public/UCLA_VAT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twwebb/Documents/python/GPT3_analogies_public/verbal_analogies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDAAD8E6-094F-DE4A-8988-8670C350EFDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60561AE9-BD51-1E43-9092-8883F72DBE33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1040" yWindow="500" windowWidth="29040" windowHeight="15840" tabRatio="852" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1132,6 +1132,7 @@
     <font>
       <sz val="9"/>
       <name val="Geneva"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1454,11 +1455,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:F81"/>
+  <dimension ref="A1:H81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
+      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1:H81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1472,7 +1473,7 @@
     <col min="7" max="16384" width="15" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>333</v>
       </c>
@@ -1491,8 +1492,10 @@
       <c r="F1" s="2" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1"/>
+      <c r="H1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>340</v>
       </c>
@@ -1511,8 +1514,10 @@
       <c r="F2" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2"/>
+      <c r="H2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="1" t="s">
         <v>90</v>
@@ -1529,8 +1534,10 @@
       <c r="F3" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3"/>
+      <c r="H3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="1" t="s">
         <v>86</v>
@@ -1547,8 +1554,10 @@
       <c r="F4" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4"/>
+      <c r="H4"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
         <v>81</v>
@@ -1565,8 +1574,10 @@
       <c r="F5" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5"/>
+      <c r="H5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
         <v>77</v>
@@ -1583,8 +1594,10 @@
       <c r="F6" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6"/>
+      <c r="H6"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
         <v>72</v>
@@ -1601,8 +1614,10 @@
       <c r="F7" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7"/>
+      <c r="H7"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
         <v>67</v>
@@ -1619,8 +1634,10 @@
       <c r="F8" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8"/>
+      <c r="H8"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
         <v>62</v>
@@ -1637,8 +1654,10 @@
       <c r="F9" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9"/>
+      <c r="H9"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
         <v>57</v>
@@ -1655,8 +1674,10 @@
       <c r="F10" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10"/>
+      <c r="H10"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
         <v>52</v>
@@ -1673,8 +1694,10 @@
       <c r="F11" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11"/>
+      <c r="H11"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
         <v>48</v>
@@ -1691,8 +1714,10 @@
       <c r="F12" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12"/>
+      <c r="H12"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
         <v>44</v>
@@ -1709,8 +1734,10 @@
       <c r="F13" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13"/>
+      <c r="H13"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
         <v>39</v>
@@ -1727,8 +1754,10 @@
       <c r="F14" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14"/>
+      <c r="H14"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
         <v>34</v>
@@ -1745,8 +1774,10 @@
       <c r="F15" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15"/>
+      <c r="H15"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
         <v>29</v>
@@ -1763,8 +1794,10 @@
       <c r="F16" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16"/>
+      <c r="H16"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
         <v>24</v>
@@ -1781,8 +1814,10 @@
       <c r="F17" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17"/>
+      <c r="H17"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
         <v>19</v>
@@ -1799,8 +1834,10 @@
       <c r="F18" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18"/>
+      <c r="H18"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
         <v>14</v>
@@ -1817,8 +1854,10 @@
       <c r="F19" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19"/>
+      <c r="H19"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
         <v>9</v>
@@ -1835,8 +1874,10 @@
       <c r="F20" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20"/>
+      <c r="H20"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
         <v>4</v>
@@ -1853,8 +1894,10 @@
       <c r="F21" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21"/>
+      <c r="H21"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>342</v>
       </c>
@@ -1873,8 +1916,10 @@
       <c r="F22" s="1" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22"/>
+      <c r="H22"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
         <v>250</v>
@@ -1891,8 +1936,10 @@
       <c r="F23" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23"/>
+      <c r="H23"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
         <v>252</v>
@@ -1909,8 +1956,10 @@
       <c r="F24" s="1" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24"/>
+      <c r="H24"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
         <v>257</v>
@@ -1927,8 +1976,10 @@
       <c r="F25" s="1" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25"/>
+      <c r="H25"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
         <v>62</v>
@@ -1945,8 +1996,10 @@
       <c r="F26" s="1" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26"/>
+      <c r="H26"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
         <v>266</v>
@@ -1963,8 +2016,10 @@
       <c r="F27" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27"/>
+      <c r="H27"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
         <v>269</v>
@@ -1981,8 +2036,10 @@
       <c r="F28" s="1" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28"/>
+      <c r="H28"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
         <v>274</v>
@@ -1999,8 +2056,10 @@
       <c r="F29" s="1" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29"/>
+      <c r="H29"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
       <c r="B30" s="1" t="s">
         <v>279</v>
@@ -2017,8 +2076,10 @@
       <c r="F30" s="1" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30"/>
+      <c r="H30"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
       <c r="B31" s="1" t="s">
         <v>284</v>
@@ -2035,8 +2096,10 @@
       <c r="F31" s="1" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31"/>
+      <c r="H31"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
       <c r="B32" s="1" t="s">
         <v>51</v>
@@ -2053,8 +2116,10 @@
       <c r="F32" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32"/>
+      <c r="H32"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
       <c r="B33" s="1" t="s">
         <v>82</v>
@@ -2071,8 +2136,10 @@
       <c r="F33" s="1" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33"/>
+      <c r="H33"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
       <c r="B34" s="1" t="s">
         <v>295</v>
@@ -2089,8 +2156,10 @@
       <c r="F34" s="1" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34"/>
+      <c r="H34"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
       <c r="B35" s="1" t="s">
         <v>300</v>
@@ -2107,8 +2176,10 @@
       <c r="F35" s="1" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G35"/>
+      <c r="H35"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
       <c r="B36" s="1" t="s">
         <v>305</v>
@@ -2125,8 +2196,10 @@
       <c r="F36" s="1" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G36"/>
+      <c r="H36"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
       <c r="B37" s="1" t="s">
         <v>310</v>
@@ -2143,8 +2216,10 @@
       <c r="F37" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G37"/>
+      <c r="H37"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
       <c r="B38" s="1" t="s">
         <v>315</v>
@@ -2161,8 +2236,10 @@
       <c r="F38" s="1" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G38"/>
+      <c r="H38"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
       <c r="B39" s="1" t="s">
         <v>29</v>
@@ -2179,8 +2256,10 @@
       <c r="F39" s="1" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G39"/>
+      <c r="H39"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
       <c r="B40" s="1" t="s">
         <v>323</v>
@@ -2197,8 +2276,10 @@
       <c r="F40" s="1" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G40"/>
+      <c r="H40"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
       <c r="B41" s="1" t="s">
         <v>328</v>
@@ -2215,8 +2296,10 @@
       <c r="F41" s="1" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G41"/>
+      <c r="H41"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>341</v>
       </c>
@@ -2235,8 +2318,10 @@
       <c r="F42" s="1" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G42"/>
+      <c r="H42"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="4"/>
       <c r="B43" s="1" t="s">
         <v>169</v>
@@ -2253,8 +2338,10 @@
       <c r="F43" s="1" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G43"/>
+      <c r="H43"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
       <c r="B44" s="1" t="s">
         <v>173</v>
@@ -2271,8 +2358,10 @@
       <c r="F44" s="1" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G44"/>
+      <c r="H44"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="4"/>
       <c r="B45" s="1" t="s">
         <v>178</v>
@@ -2289,8 +2378,10 @@
       <c r="F45" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G45"/>
+      <c r="H45"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="4"/>
       <c r="B46" s="1" t="s">
         <v>182</v>
@@ -2307,8 +2398,10 @@
       <c r="F46" s="1" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G46"/>
+      <c r="H46"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="4"/>
       <c r="B47" s="1" t="s">
         <v>187</v>
@@ -2325,8 +2418,10 @@
       <c r="F47" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G47"/>
+      <c r="H47"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="4"/>
       <c r="B48" s="1" t="s">
         <v>191</v>
@@ -2343,8 +2438,10 @@
       <c r="F48" s="1" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G48"/>
+      <c r="H48"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="4"/>
       <c r="B49" s="1" t="s">
         <v>195</v>
@@ -2361,8 +2458,10 @@
       <c r="F49" s="1" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G49"/>
+      <c r="H49"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="4"/>
       <c r="B50" s="1" t="s">
         <v>200</v>
@@ -2379,8 +2478,10 @@
       <c r="F50" s="1" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G50"/>
+      <c r="H50"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="4"/>
       <c r="B51" s="1" t="s">
         <v>204</v>
@@ -2397,8 +2498,10 @@
       <c r="F51" s="1" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G51"/>
+      <c r="H51"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="4"/>
       <c r="B52" s="1" t="s">
         <v>208</v>
@@ -2415,8 +2518,10 @@
       <c r="F52" s="1" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G52"/>
+      <c r="H52"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="4"/>
       <c r="B53" s="1" t="s">
         <v>213</v>
@@ -2433,8 +2538,10 @@
       <c r="F53" s="1" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G53"/>
+      <c r="H53"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="4"/>
       <c r="B54" s="1" t="s">
         <v>184</v>
@@ -2451,8 +2558,10 @@
       <c r="F54" s="1" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G54"/>
+      <c r="H54"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="4"/>
       <c r="B55" s="1" t="s">
         <v>221</v>
@@ -2469,8 +2578,10 @@
       <c r="F55" s="1" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G55"/>
+      <c r="H55"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="4"/>
       <c r="B56" s="1" t="s">
         <v>225</v>
@@ -2487,8 +2598,10 @@
       <c r="F56" s="1" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G56"/>
+      <c r="H56"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="4"/>
       <c r="B57" s="1" t="s">
         <v>230</v>
@@ -2505,8 +2618,10 @@
       <c r="F57" s="1" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G57"/>
+      <c r="H57"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="4"/>
       <c r="B58" s="1" t="s">
         <v>234</v>
@@ -2523,8 +2638,10 @@
       <c r="F58" s="1" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G58"/>
+      <c r="H58"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="4"/>
       <c r="B59" s="1" t="s">
         <v>175</v>
@@ -2541,8 +2658,10 @@
       <c r="F59" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G59"/>
+      <c r="H59"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="4"/>
       <c r="B60" s="1" t="s">
         <v>200</v>
@@ -2559,8 +2678,10 @@
       <c r="F60" s="1" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G60"/>
+      <c r="H60"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="4"/>
       <c r="B61" s="1" t="s">
         <v>175</v>
@@ -2577,8 +2698,10 @@
       <c r="F61" s="1" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G61"/>
+      <c r="H61"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>343</v>
       </c>
@@ -2597,8 +2720,10 @@
       <c r="F62" s="1" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G62"/>
+      <c r="H62"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="4"/>
       <c r="B63" s="1" t="s">
         <v>154</v>
@@ -2615,8 +2740,10 @@
       <c r="F63" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G63"/>
+      <c r="H63"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="4"/>
       <c r="B64" s="1" t="s">
         <v>110</v>
@@ -2633,8 +2760,10 @@
       <c r="F64" s="1" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G64"/>
+      <c r="H64"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="4"/>
       <c r="B65" s="1" t="s">
         <v>106</v>
@@ -2651,8 +2780,10 @@
       <c r="F65" s="1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G65"/>
+      <c r="H65"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="4"/>
       <c r="B66" s="1" t="s">
         <v>96</v>
@@ -2669,8 +2800,10 @@
       <c r="F66" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G66"/>
+      <c r="H66"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="4"/>
       <c r="B67" s="1" t="s">
         <v>115</v>
@@ -2687,8 +2820,10 @@
       <c r="F67" s="1" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G67"/>
+      <c r="H67"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="4"/>
       <c r="B68" s="1" t="s">
         <v>113</v>
@@ -2705,8 +2840,10 @@
       <c r="F68" s="1" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G68"/>
+      <c r="H68"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="4"/>
       <c r="B69" s="1" t="s">
         <v>115</v>
@@ -2723,8 +2860,10 @@
       <c r="F69" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G69"/>
+      <c r="H69"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="4"/>
       <c r="B70" s="1" t="s">
         <v>104</v>
@@ -2741,8 +2880,10 @@
       <c r="F70" s="1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G70"/>
+      <c r="H70"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="4"/>
       <c r="B71" s="1" t="s">
         <v>119</v>
@@ -2759,8 +2900,10 @@
       <c r="F71" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G71"/>
+      <c r="H71"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="4"/>
       <c r="B72" s="1" t="s">
         <v>99</v>
@@ -2777,8 +2920,10 @@
       <c r="F72" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G72"/>
+      <c r="H72"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="4"/>
       <c r="B73" s="1" t="s">
         <v>101</v>
@@ -2795,8 +2940,10 @@
       <c r="F73" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G73"/>
+      <c r="H73"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="4"/>
       <c r="B74" s="1" t="s">
         <v>128</v>
@@ -2813,8 +2960,10 @@
       <c r="F74" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G74"/>
+      <c r="H74"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="4"/>
       <c r="B75" s="1" t="s">
         <v>101</v>
@@ -2831,8 +2980,10 @@
       <c r="F75" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G75"/>
+      <c r="H75"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="4"/>
       <c r="B76" s="1" t="s">
         <v>110</v>
@@ -2849,8 +3000,10 @@
       <c r="F76" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G76"/>
+      <c r="H76"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="4"/>
       <c r="B77" s="1" t="s">
         <v>106</v>
@@ -2867,8 +3020,10 @@
       <c r="F77" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G77"/>
+      <c r="H77"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="4"/>
       <c r="B78" s="1" t="s">
         <v>113</v>
@@ -2885,8 +3040,10 @@
       <c r="F78" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G78"/>
+      <c r="H78"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="4"/>
       <c r="B79" s="1" t="s">
         <v>99</v>
@@ -2903,8 +3060,10 @@
       <c r="F79" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G79"/>
+      <c r="H79"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="4"/>
       <c r="B80" s="1" t="s">
         <v>104</v>
@@ -2921,8 +3080,10 @@
       <c r="F80" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G80"/>
+      <c r="H80"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="4"/>
       <c r="B81" s="1" t="s">
         <v>99</v>
@@ -2939,6 +3100,8 @@
       <c r="F81" s="1" t="s">
         <v>95</v>
       </c>
+      <c r="G81"/>
+      <c r="H81"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>